<commit_message>
Restored Debug and Release builds.  Restored startup banner.  Added parameter descriptions.
</commit_message>
<xml_diff>
--- a/Thunderboard Demo.xlsx
+++ b/Thunderboard Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\SimplicityStudio\v5_workspace\reach-silabs-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck.peplinski\cygnus\reach-silabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD77CFFC-D133-401A-A1F5-C0B7C520A9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39601A96-6891-49A6-B090-909619A7278B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4608" yWindow="4608" windowWidth="34560" windowHeight="18648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
   <si>
     <t>Device Name</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>int32</t>
-  </si>
-  <si>
-    <t>The offset from UTC</t>
   </si>
   <si>
     <t>seconds</t>
@@ -262,6 +259,21 @@
   </si>
   <si>
     <t>Click for Wisdom</t>
+  </si>
+  <si>
+    <t>Read from Thunderboard Sensor</t>
+  </si>
+  <si>
+    <t>Read from Thunderboard</t>
+  </si>
+  <si>
+    <t>Controls command line color</t>
+  </si>
+  <si>
+    <t>(Time service)</t>
+  </si>
+  <si>
+    <t>(Time service) Offset from UTC</t>
   </si>
 </sst>
 </file>
@@ -564,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,11 +646,11 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z136"/>
+  <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -648,7 +660,7 @@
     <col min="7" max="7" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -683,7 +695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -721,158 +733,166 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
-      <c r="H4" s="4">
-        <v>-43200</v>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>35</v>
       </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>43200</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4">
-        <v>6</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>39</v>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
       </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="H7" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>60</v>
+      </c>
       <c r="K7" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -880,276 +900,294 @@
         <v>25</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>7</v>
+      </c>
       <c r="K9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
-      <c r="H10" s="4">
-        <v>0.01</v>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
+        <v>35</v>
       </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4">
-        <v>60</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4">
-        <v>0</v>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>35</v>
       </c>
-      <c r="J11" s="4">
-        <v>7</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="4">
-        <v>0</v>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
+        <v>35</v>
       </c>
-      <c r="J12" s="4">
-        <v>7</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>59</v>
+      <c r="D13" s="4" t="s">
+        <v>78</v>
       </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E14" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E15" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="E17" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>71</v>
+      <c r="D18" s="4" t="s">
+        <v>81</v>
       </c>
+      <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="H19" s="4">
+        <v>-43200</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>43200</v>
+      </c>
       <c r="K19" s="4" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>71</v>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4">
+        <v>6</v>
       </c>
-      <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1162,7 +1200,7 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1175,7 +1213,7 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1188,7 +1226,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1201,7 +1239,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1214,7 +1252,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1227,7 +1265,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1240,7 +1278,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1253,7 +1291,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1266,7 +1304,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1279,7 +1317,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1292,7 +1330,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1305,7 +1343,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1318,7 +1356,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1331,7 +1369,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1344,7 +1382,7 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1357,7 +1395,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1370,7 +1408,7 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1383,7 +1421,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1396,7 +1434,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1409,7 +1447,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1422,7 +1460,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1435,7 +1473,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1448,7 +1486,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1461,7 +1499,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1474,7 +1512,7 @@
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1487,7 +1525,7 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1500,7 +1538,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1513,7 +1551,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1526,7 +1564,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1539,7 +1577,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1552,7 +1590,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1565,7 +1603,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1578,7 +1616,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1591,7 +1629,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1604,7 +1642,7 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1617,7 +1655,7 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1630,7 +1668,7 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1643,7 +1681,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1656,7 +1694,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1669,7 +1707,7 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1682,7 +1720,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1695,7 +1733,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1708,7 +1746,7 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1721,7 +1759,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1734,7 +1772,7 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1747,7 +1785,7 @@
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1760,7 +1798,7 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1773,7 +1811,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1786,7 +1824,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -1799,7 +1837,7 @@
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -1812,7 +1850,7 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -1825,7 +1863,7 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -1838,7 +1876,7 @@
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -1851,7 +1889,7 @@
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -1864,7 +1902,7 @@
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -1877,7 +1915,7 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -1890,7 +1928,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -1903,7 +1941,7 @@
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -1916,7 +1954,7 @@
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -1929,7 +1967,7 @@
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -1942,7 +1980,7 @@
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -1955,7 +1993,7 @@
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -1968,7 +2006,7 @@
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -1981,7 +2019,7 @@
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -1994,7 +2032,7 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2007,46 +2045,46 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
+      <c r="F87" s="5"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="5"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
+      <c r="F89" s="5"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2059,46 +2097,46 @@
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
-      <c r="F91" s="5"/>
+      <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
-      <c r="F92" s="5"/>
+      <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
-      <c r="F93" s="5"/>
+      <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2111,7 +2149,7 @@
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -2124,7 +2162,7 @@
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -2137,7 +2175,7 @@
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -2150,7 +2188,7 @@
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -2163,7 +2201,7 @@
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -2176,7 +2214,7 @@
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -2189,46 +2227,46 @@
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
-      <c r="F101" s="4"/>
+      <c r="F101" s="5"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
-      <c r="F102" s="4"/>
+      <c r="F102" s="5"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
+      <c r="F103" s="5"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -2241,7 +2279,7 @@
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -2254,7 +2292,7 @@
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -2267,7 +2305,7 @@
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -2280,7 +2318,7 @@
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -2293,7 +2331,7 @@
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -2306,7 +2344,7 @@
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -2319,7 +2357,7 @@
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -2332,7 +2370,7 @@
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -2345,7 +2383,7 @@
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -2358,7 +2396,7 @@
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -2371,7 +2409,7 @@
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -2384,7 +2422,7 @@
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -2397,7 +2435,7 @@
       <c r="J116" s="4"/>
       <c r="K116" s="4"/>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -2409,8 +2447,23 @@
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
-    </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L117" s="4"/>
+      <c r="M117" s="4"/>
+      <c r="N117" s="4"/>
+      <c r="O117" s="4"/>
+      <c r="P117" s="4"/>
+      <c r="Q117" s="4"/>
+      <c r="R117" s="4"/>
+      <c r="S117" s="4"/>
+      <c r="T117" s="4"/>
+      <c r="U117" s="4"/>
+      <c r="V117" s="4"/>
+      <c r="W117" s="4"/>
+      <c r="X117" s="4"/>
+      <c r="Y117" s="4"/>
+      <c r="Z117" s="4"/>
+    </row>
+    <row r="118" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -2422,77 +2475,62 @@
       <c r="I118" s="4"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
-    </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="4"/>
+      <c r="W118" s="4"/>
+      <c r="X118" s="4"/>
+      <c r="Y118" s="4"/>
+      <c r="Z118" s="4"/>
+    </row>
+    <row r="119" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
-      <c r="F119" s="5"/>
+      <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
       <c r="J119" s="4"/>
       <c r="K119" s="4"/>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
-      <c r="F120" s="5"/>
+      <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
       <c r="J120" s="4"/>
       <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-      <c r="S120" s="4"/>
-      <c r="T120" s="4"/>
-      <c r="U120" s="4"/>
-      <c r="V120" s="4"/>
-      <c r="W120" s="4"/>
-      <c r="X120" s="4"/>
-      <c r="Y120" s="4"/>
-      <c r="Z120" s="4"/>
-    </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
-      <c r="F121" s="5"/>
+      <c r="F121" s="4"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
       <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-      <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-      <c r="S121" s="4"/>
-      <c r="T121" s="4"/>
-      <c r="U121" s="4"/>
-      <c r="V121" s="4"/>
-      <c r="W121" s="4"/>
-      <c r="X121" s="4"/>
-      <c r="Y121" s="4"/>
-      <c r="Z121" s="4"/>
-    </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -2505,7 +2543,7 @@
       <c r="J122" s="4"/>
       <c r="K122" s="4"/>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -2518,7 +2556,7 @@
       <c r="J123" s="4"/>
       <c r="K123" s="4"/>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -2531,7 +2569,7 @@
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -2544,7 +2582,7 @@
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -2557,7 +2595,7 @@
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -2570,7 +2608,7 @@
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -2583,7 +2621,7 @@
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -2596,7 +2634,7 @@
       <c r="J129" s="4"/>
       <c r="K129" s="4"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -2609,7 +2647,7 @@
       <c r="J130" s="4"/>
       <c r="K130" s="4"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -2622,7 +2660,7 @@
       <c r="J131" s="4"/>
       <c r="K131" s="4"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -2635,7 +2673,7 @@
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -2648,66 +2686,27 @@
       <c r="J133" s="4"/>
       <c r="K133" s="4"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="4"/>
-      <c r="E134" s="4"/>
-      <c r="F134" s="4"/>
-      <c r="G134" s="4"/>
-      <c r="H134" s="4"/>
-      <c r="I134" s="4"/>
-      <c r="J134" s="4"/>
-      <c r="K134" s="4"/>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="4"/>
-      <c r="K135" s="4"/>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A136" s="4"/>
-      <c r="B136" s="4"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
-      <c r="E136" s="4"/>
-      <c r="F136" s="4"/>
-      <c r="G136" s="4"/>
-      <c r="H136" s="4"/>
-      <c r="I136" s="4"/>
-      <c r="J136" s="4"/>
-      <c r="K136" s="4"/>
-    </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B8 B9:B1048576" xr:uid="{92D4FE4B-E0B5-4787-81EA-AD354F206254}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2 B3:B1048576" xr:uid="{92D4FE4B-E0B5-4787-81EA-AD354F206254}">
       <formula1>"uint32,int32,float32,uint64,int64,bool,string,enum,bitfield,bytes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G8 G9:G1048576" xr:uid="{7D79F860-15AF-4A9A-97D7-333719CADA47}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2 G3:G1048576" xr:uid="{7D79F860-15AF-4A9A-97D7-333719CADA47}">
       <formula1>"None,Read,Write,Read/Write"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2:K8 K9:K1048576" xr:uid="{50AA6DF0-BD9D-44F2-B835-5333D9081C56}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2 K3:K1048576" xr:uid="{50AA6DF0-BD9D-44F2-B835-5333D9081C56}">
       <formula1>"RAM,NVM,Extended RAM,Extended NVM"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Descriptions must be less than 32 characters." sqref="D2:D8 D9:D1048576" xr:uid="{7CCC57C2-5432-4C01-863D-D130673DEC89}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Descriptions must be less than 32 characters." sqref="D2 D3:D1048576" xr:uid="{7CCC57C2-5432-4C01-863D-D130673DEC89}">
       <formula1>32</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Units must be less than 16 characters." sqref="E2:E8 E9:E1048576" xr:uid="{D948516B-1800-4D22-90D0-C9DAC274F264}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Units must be less than 16 characters." sqref="E2 E3:E1048576" xr:uid="{D948516B-1800-4D22-90D0-C9DAC274F264}">
       <formula1>16</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Buffer Size Exceeded" error="Bytearrays can only store up to 32 bytes." sqref="F2:F8 F9:F1048576" xr:uid="{0C8CCC3B-6309-42BB-8DA3-49CD4D0ECF06}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Buffer Size Exceeded" error="Bytearrays can only store up to 32 bytes." sqref="F2 F3:F1048576" xr:uid="{0C8CCC3B-6309-42BB-8DA3-49CD4D0ECF06}">
       <formula1>32</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Names must be less than 24 characters." sqref="A2:A8 A9:A1048576" xr:uid="{DF41DA1D-DAC2-4212-B177-2AD51C0776F2}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Names must be less than 24 characters." sqref="A2 A3:A1048576" xr:uid="{DF41DA1D-DAC2-4212-B177-2AD51C0776F2}">
       <formula1>24</formula1>
     </dataValidation>
   </dataValidations>
@@ -2748,7 +2747,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4">
         <v>512</v>
@@ -2762,13 +2761,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4">
         <v>17900</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -7781,8 +7780,8 @@
   </sheetPr>
   <dimension ref="A1:B993"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7800,15 +7799,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -10823,49 +10822,49 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4"/>
     </row>
@@ -13883,19 +13882,19 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updates to match reach-util and new reach-c-stack changes, and improvements to Doxygen comments
</commit_message>
<xml_diff>
--- a/Thunderboard Demo.xlsx
+++ b/Thunderboard Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck.peplinski\cygnus\reach-silabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reach-silabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39601A96-6891-49A6-B090-909619A7278B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77839339-1544-4912-8EB8-65A4338BB28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4608" yWindow="4608" windowWidth="34560" windowHeight="18648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
   <si>
     <t>Device Name</t>
   </si>
@@ -275,12 +275,18 @@
   <si>
     <t>(Time service) Offset from UTC</t>
   </si>
+  <si>
+    <t>Require Checksum</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -292,12 +298,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,11 +313,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -341,6 +359,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,7 +667,7 @@
   </sheetPr>
   <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
@@ -2720,10 +2739,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D997"/>
+  <dimension ref="A1:E997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2731,7 +2750,7 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2744,8 +2763,11 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -2758,8 +2780,11 @@
       <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -2772,78 +2797,81 @@
       <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -7754,7 +7782,7 @@
       <c r="D997" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{A696E6F1-CBCD-4A0E-B7A6-D8DC2BE4F268}">
       <formula1>0</formula1>
     </dataValidation>
@@ -7766,6 +7794,9 @@
     </dataValidation>
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Names must be less than 24 characters." sqref="A2:A1048576" xr:uid="{DCEF0DBD-40DA-42A4-B1BB-6C9E36FCEB02}">
       <formula1>24</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{E91C9F5B-FC5B-48DF-AE0D-F7E6EEF4F99D}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Locally defined notifications can be enabled and disabled with commands.  This is a necessary step toward reporting notification configuration to the client.
</commit_message>
<xml_diff>
--- a/Thunderboard Demo.xlsx
+++ b/Thunderboard Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.peplinski\Reach\reach-silabs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck.peplinski\cygnus\reach-silabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77839339-1544-4912-8EB8-65A4338BB28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5C885-CDF2-4459-9AE6-11B3166D6915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8004" yWindow="3120" windowWidth="28644" windowHeight="11220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>Device Name</t>
   </si>
@@ -281,12 +281,57 @@
   <si>
     <t>No</t>
   </si>
+  <si>
+    <t>Notify</t>
+  </si>
+  <si>
+    <t>min period</t>
+  </si>
+  <si>
+    <t>max period</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>No Logging</t>
+  </si>
+  <si>
+    <t>Much Logging</t>
+  </si>
+  <si>
+    <t>Notifications On</t>
+  </si>
+  <si>
+    <t>Notifications Off</t>
+  </si>
+  <si>
+    <t>lm 0</t>
+  </si>
+  <si>
+    <t>lm 1c7</t>
+  </si>
+  <si>
+    <t>remote CLI On</t>
+  </si>
+  <si>
+    <t>remote CLI Off</t>
+  </si>
+  <si>
+    <t>Echo CLI to remote (expensive)</t>
+  </si>
+  <si>
+    <t>Do not echo CLI to remote</t>
+  </si>
+  <si>
+    <t>Toggles Identify</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -329,6 +374,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -350,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,6 +416,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,9 +725,9 @@
   </sheetPr>
   <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -736,10 +794,10 @@
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -784,7 +842,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -953,6 +1011,18 @@
       <c r="K10" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>100</v>
+      </c>
+      <c r="N10">
+        <v>60000</v>
+      </c>
+      <c r="O10">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -978,6 +1048,18 @@
       <c r="K11" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+      <c r="N11">
+        <v>60000</v>
+      </c>
+      <c r="O11">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1003,6 +1085,18 @@
       <c r="K12" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+      <c r="N12">
+        <v>60000</v>
+      </c>
+      <c r="O12">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1026,6 +1120,18 @@
       <c r="K13" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>60000</v>
+      </c>
+      <c r="O13">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1051,6 +1157,18 @@
       <c r="K14" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>100</v>
+      </c>
+      <c r="N14">
+        <v>60000</v>
+      </c>
+      <c r="O14">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -1076,6 +1194,18 @@
       <c r="K15" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>100</v>
+      </c>
+      <c r="N15">
+        <v>60000</v>
+      </c>
+      <c r="O15">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1101,8 +1231,20 @@
       <c r="K16" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="L16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="N16">
+        <v>60000</v>
+      </c>
+      <c r="O16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>69</v>
       </c>
@@ -1126,8 +1268,20 @@
       <c r="K17" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+      <c r="N17">
+        <v>60000</v>
+      </c>
+      <c r="O17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1152,7 +1306,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -1183,7 +1337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1206,7 +1360,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1218,8 +1372,20 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="L21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1232,7 +1398,7 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1245,7 +1411,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1258,7 +1424,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1271,7 +1437,7 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1284,7 +1450,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1297,7 +1463,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1310,7 +1476,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1323,7 +1489,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1336,7 +1502,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1349,7 +1515,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2466,10 +2632,10 @@
       <c r="I117" s="4"/>
       <c r="J117" s="4"/>
       <c r="K117" s="4"/>
-      <c r="L117" s="4"/>
-      <c r="M117" s="4"/>
-      <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
+      <c r="L117" s="8"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="8"/>
+      <c r="O117" s="8"/>
       <c r="P117" s="4"/>
       <c r="Q117" s="4"/>
       <c r="R117" s="4"/>
@@ -2494,10 +2660,10 @@
       <c r="I118" s="4"/>
       <c r="J118" s="4"/>
       <c r="K118" s="4"/>
-      <c r="L118" s="4"/>
-      <c r="M118" s="4"/>
-      <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
+      <c r="L118" s="8"/>
+      <c r="M118" s="8"/>
+      <c r="N118" s="8"/>
+      <c r="O118" s="8"/>
       <c r="P118" s="4"/>
       <c r="Q118" s="4"/>
       <c r="R118" s="4"/>
@@ -2707,25 +2873,25 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2 B3:B1048576" xr:uid="{92D4FE4B-E0B5-4787-81EA-AD354F206254}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{92D4FE4B-E0B5-4787-81EA-AD354F206254}">
       <formula1>"uint32,int32,float32,uint64,int64,bool,string,enum,bitfield,bytes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2 G3:G1048576" xr:uid="{7D79F860-15AF-4A9A-97D7-333719CADA47}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{7D79F860-15AF-4A9A-97D7-333719CADA47}">
       <formula1>"None,Read,Write,Read/Write"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2 K3:K1048576" xr:uid="{50AA6DF0-BD9D-44F2-B835-5333D9081C56}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{50AA6DF0-BD9D-44F2-B835-5333D9081C56}">
       <formula1>"RAM,NVM,Extended RAM,Extended NVM"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Descriptions must be less than 32 characters." sqref="D2 D3:D1048576" xr:uid="{7CCC57C2-5432-4C01-863D-D130673DEC89}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Descriptions must be less than 32 characters." sqref="D2:D1048576" xr:uid="{7CCC57C2-5432-4C01-863D-D130673DEC89}">
       <formula1>32</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Units must be less than 16 characters." sqref="E2 E3:E1048576" xr:uid="{D948516B-1800-4D22-90D0-C9DAC274F264}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Units must be less than 16 characters." sqref="E2:E1048576" xr:uid="{D948516B-1800-4D22-90D0-C9DAC274F264}">
       <formula1>16</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Buffer Size Exceeded" error="Bytearrays can only store up to 32 bytes." sqref="F2 F3:F1048576" xr:uid="{0C8CCC3B-6309-42BB-8DA3-49CD4D0ECF06}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Buffer Size Exceeded" error="Bytearrays can only store up to 32 bytes." sqref="F2:F1048576" xr:uid="{0C8CCC3B-6309-42BB-8DA3-49CD4D0ECF06}">
       <formula1>32</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Names must be less than 24 characters." sqref="A2 A3:A1048576" xr:uid="{DF41DA1D-DAC2-4212-B177-2AD51C0776F2}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Character limit exceeded" error="Names must be less than 24 characters." sqref="A2:A1048576" xr:uid="{DF41DA1D-DAC2-4212-B177-2AD51C0776F2}">
       <formula1>24</formula1>
     </dataValidation>
   </dataValidations>
@@ -2741,7 +2907,7 @@
   </sheetPr>
   <dimension ref="A1:E997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7812,7 +7978,7 @@
   <dimension ref="A1:B993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7843,28 +8009,48 @@
       <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>

</xml_diff>

<commit_message>
Added a third file (dev_null) that goes nowhere and produces junk to be used for speed testing.
</commit_message>
<xml_diff>
--- a/Thunderboard Demo.xlsx
+++ b/Thunderboard Demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck.peplinski\cygnus\reach-silabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5C885-CDF2-4459-9AE6-11B3166D6915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9E96C0-9B8E-4E4C-BA59-ACCB8771D45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8004" yWindow="3120" windowWidth="28644" windowHeight="11220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8004" yWindow="3120" windowWidth="28644" windowHeight="11220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="101">
   <si>
     <t>Device Name</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Toggles Identify</t>
+  </si>
+  <si>
+    <t>dev_null</t>
   </si>
 </sst>
 </file>
@@ -725,7 +728,7 @@
   </sheetPr>
   <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
@@ -2907,8 +2910,8 @@
   </sheetPr>
   <dimension ref="A1:E997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2968,10 +2971,21 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>

</xml_diff>

<commit_message>
Updated code gen in reach-util to match the latest access control.  Regenerated definitions.c
</commit_message>
<xml_diff>
--- a/Thunderboard Demo.xlsx
+++ b/Thunderboard Demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuck.peplinski\cygnus\reach-silabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9E96C0-9B8E-4E4C-BA59-ACCB8771D45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15F580C-2E8A-4A54-9DFF-822EB0080853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8004" yWindow="3120" windowWidth="28644" windowHeight="11220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12636" yWindow="6072" windowWidth="27996" windowHeight="18600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device Information" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
   <si>
     <t>Device Name</t>
   </si>
@@ -329,6 +329,9 @@
   <si>
     <t>dev_null</t>
   </si>
+  <si>
+    <t>Max Size</t>
+  </si>
 </sst>
 </file>
 
@@ -382,11 +385,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -421,6 +426,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,9 +742,9 @@
   </sheetPr>
   <dimension ref="A1:Z133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -738,41 +752,54 @@
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:26" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
@@ -1375,18 +1402,10 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>88</v>
-      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
@@ -2908,10 +2927,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E997"/>
+  <dimension ref="A1:F997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2919,7 +2938,7 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2935,8 +2954,11 @@
       <c r="E1" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -2952,8 +2974,11 @@
       <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -2969,13 +2994,16 @@
       <c r="E3" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4">
+        <v>17900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B4" s="4">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
@@ -2986,72 +3014,75 @@
       <c r="E4" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -7963,7 +7994,7 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{A696E6F1-CBCD-4A0E-B7A6-D8DC2BE4F268}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576 F3:F4" xr:uid="{A696E6F1-CBCD-4A0E-B7A6-D8DC2BE4F268}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{B4A9057C-0490-4C7A-AD27-4B4DDBCECFFF}">

</xml_diff>